<commit_message>
Implemented experiment run tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmineleblond-chartrand/c3g/freezeman/backend/fms_core/static/submission_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990515B1-AB64-4C48-9267-D2D0788514F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A771FB8-94DA-4F42-9DC7-B697A7E6A7AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1760" windowWidth="25080" windowHeight="12980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1760" windowWidth="25080" windowHeight="12980" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -1101,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -5153,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMI19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5209,7 +5209,7 @@
         <v>106</v>
       </c>
       <c r="D5">
-        <v>5000</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Template importer Experiment Run tests (#157)
* Implemented experiment run tests

* Continued tests and fixed property values bien created with None values

* Finished tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmineleblond-chartrand/c3g/freezeman/backend/fms_core/static/submission_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990515B1-AB64-4C48-9267-D2D0788514F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A771FB8-94DA-4F42-9DC7-B697A7E6A7AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1760" windowWidth="25080" windowHeight="12980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1760" windowWidth="25080" windowHeight="12980" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -1101,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -5153,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMI19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5209,7 +5209,7 @@
         <v>106</v>
       </c>
       <c r="D5">
-        <v>5000</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Changes to add experiment run name to the backend and frontend and list multiple templates.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_Infinium_24_vtest.xlsx
@@ -205,7 +205,7 @@
     <t xml:space="preserve">Image (scan)</t>
   </si>
   <si>
-    <t xml:space="preserve">Experiment ID</t>
+    <t xml:space="preserve">Experiment Name</t>
   </si>
   <si>
     <t xml:space="preserve">Experiment Container Barcode</t>
@@ -1906,7 +1906,7 @@
   <dimension ref="A1:AMI106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5869,7 +5869,7 @@
   <dimension ref="A1:AMH19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5954,7 +5954,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.53"/>

</xml_diff>